<commit_message>
comitting to pull from mac
</commit_message>
<xml_diff>
--- a/M0.5D0.001E0.99A0.99_200x200_first_cluster.xlsx
+++ b/M0.5D0.001E0.99A0.99_200x200_first_cluster.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,6 +458,32 @@
         <v>94960001</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>00000398</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>22300001</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>00000399</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>117640001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>